<commit_message>
Spring 2024 updated plan
</commit_message>
<xml_diff>
--- a/lecturePlan.xlsx
+++ b/lecturePlan.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23127"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s15052\Documents\Teaching\BAN430\BAN430_book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD16530C-6427-44E2-858F-B7D7CCA23CA7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9615B9EA-DD64-495A-8B60-6412B620A873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="12735" activeTab="2" xr2:uid="{DEDCCCE6-C2B3-4C3C-BD8B-2E3EEC4135F8}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="2" xr2:uid="{DEDCCCE6-C2B3-4C3C-BD8B-2E3EEC4135F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="94">
   <si>
     <t>Week number</t>
   </si>
@@ -221,84 +221,6 @@
     <t>Dynamic regresion models</t>
   </si>
   <si>
-    <t>16.01.2023</t>
-  </si>
-  <si>
-    <t>19.01.2023</t>
-  </si>
-  <si>
-    <t>23.01.2023</t>
-  </si>
-  <si>
-    <t>26.01.2023</t>
-  </si>
-  <si>
-    <t>30.01.2023</t>
-  </si>
-  <si>
-    <t>02.02.2023</t>
-  </si>
-  <si>
-    <t>06.02.2023</t>
-  </si>
-  <si>
-    <t>09.02.2023</t>
-  </si>
-  <si>
-    <t>13.02.2023</t>
-  </si>
-  <si>
-    <t>16.02.2023</t>
-  </si>
-  <si>
-    <t>20.02.2023</t>
-  </si>
-  <si>
-    <t>23.02.2023</t>
-  </si>
-  <si>
-    <t>27.02.2023</t>
-  </si>
-  <si>
-    <t>02.03.2023</t>
-  </si>
-  <si>
-    <t>06.03.2023</t>
-  </si>
-  <si>
-    <t>09.03.2023</t>
-  </si>
-  <si>
-    <t>13.03.2023</t>
-  </si>
-  <si>
-    <t>16.03.2023</t>
-  </si>
-  <si>
-    <t>20.03.2023</t>
-  </si>
-  <si>
-    <t>03.04.2023</t>
-  </si>
-  <si>
-    <t>06.04.2023</t>
-  </si>
-  <si>
-    <t>27.03.2023</t>
-  </si>
-  <si>
-    <t>30.03.2023</t>
-  </si>
-  <si>
-    <t>13.04.2023</t>
-  </si>
-  <si>
-    <t>10.04.2023</t>
-  </si>
-  <si>
-    <t>08.05.2023</t>
-  </si>
-  <si>
     <t>Introduction lecture</t>
   </si>
   <si>
@@ -308,9 +230,6 @@
     <t>No lecture: Selfstudy judgmental forecasts (website)</t>
   </si>
   <si>
-    <t>23.03.2023</t>
-  </si>
-  <si>
     <t>ARIMA + Dynamic regression models</t>
   </si>
   <si>
@@ -318,12 +237,93 @@
   </si>
   <si>
     <t>Solutions to Workshop 2</t>
+  </si>
+  <si>
+    <t>24.04.2024</t>
+  </si>
+  <si>
+    <t>15.01.2024</t>
+  </si>
+  <si>
+    <t>18.01.2024</t>
+  </si>
+  <si>
+    <t>22.01.2024</t>
+  </si>
+  <si>
+    <t>25.01.2024</t>
+  </si>
+  <si>
+    <t>29.01.2024</t>
+  </si>
+  <si>
+    <t>01.02.2024</t>
+  </si>
+  <si>
+    <t>05.02.2024</t>
+  </si>
+  <si>
+    <t>08.02.2024</t>
+  </si>
+  <si>
+    <t>12.02.2024</t>
+  </si>
+  <si>
+    <t>15.02.2024</t>
+  </si>
+  <si>
+    <t>19.02.2024</t>
+  </si>
+  <si>
+    <t>22.02.2024</t>
+  </si>
+  <si>
+    <t>26.02.2024</t>
+  </si>
+  <si>
+    <t>29.02.2024</t>
+  </si>
+  <si>
+    <t>11.03.2024</t>
+  </si>
+  <si>
+    <t>04.03.024</t>
+  </si>
+  <si>
+    <t>07.03.2024</t>
+  </si>
+  <si>
+    <t>14.03.2024</t>
+  </si>
+  <si>
+    <t>21.03.2024</t>
+  </si>
+  <si>
+    <t>18.03.2024</t>
+  </si>
+  <si>
+    <t>28.03.2024</t>
+  </si>
+  <si>
+    <t>25.03.2024</t>
+  </si>
+  <si>
+    <t>04.04.2024</t>
+  </si>
+  <si>
+    <t>01.04.2024</t>
+  </si>
+  <si>
+    <t>11.04.2024</t>
+  </si>
+  <si>
+    <t>08.04.2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -584,10 +584,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="99">
+  <cellXfs count="100">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="14" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -686,12 +685,6 @@
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -701,68 +694,29 @@
     <xf numFmtId="49" fontId="0" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="6" fillId="4" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="4" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="49" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -848,12 +802,63 @@
     <xf numFmtId="49" fontId="9" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="1" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="49" fontId="5" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="49" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{08A62E74-7142-47AC-89E9-0DC02D7C47DC}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1280,13 +1285,13 @@
       <c r="A7">
         <v>8</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" t="s">
         <v>8</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" t="s">
         <v>8</v>
       </c>
     </row>
@@ -1319,13 +1324,13 @@
       <c r="A10">
         <v>11</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" t="s">
         <v>10</v>
       </c>
     </row>
@@ -1393,8 +1398,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF6C382B-A390-441B-AFA9-C1DFECC0D308}">
   <dimension ref="A1:H50"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17:C48"/>
+    <sheetView topLeftCell="A14" workbookViewId="0">
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1453,10 +1458,10 @@
       <c r="F2" t="s">
         <v>33</v>
       </c>
-      <c r="G2" s="3">
+      <c r="G2" s="2">
         <v>44942</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <v>44945</v>
       </c>
     </row>
@@ -1473,10 +1478,10 @@
       <c r="D3" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="3">
+      <c r="G3" s="2">
         <v>44949</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <v>44952</v>
       </c>
     </row>
@@ -1496,10 +1501,10 @@
       <c r="E4" t="s">
         <v>4</v>
       </c>
-      <c r="G4" s="3">
+      <c r="G4" s="2">
         <v>44956</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <v>44959</v>
       </c>
     </row>
@@ -1519,10 +1524,10 @@
       <c r="E5" t="s">
         <v>7</v>
       </c>
-      <c r="G5" s="3">
+      <c r="G5" s="2">
         <v>44963</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <v>44966</v>
       </c>
     </row>
@@ -1530,22 +1535,22 @@
       <c r="A6">
         <v>8</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>8</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" t="s">
         <v>8</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="3">
+      <c r="G6" s="2">
         <v>44970</v>
       </c>
-      <c r="H6" s="3">
+      <c r="H6" s="2">
         <v>44973</v>
       </c>
     </row>
@@ -1565,10 +1570,10 @@
       <c r="F7" t="s">
         <v>29</v>
       </c>
-      <c r="G7" s="4">
+      <c r="G7" s="3">
         <v>44977</v>
       </c>
-      <c r="H7" s="4">
+      <c r="H7" s="3">
         <v>44980</v>
       </c>
     </row>
@@ -1585,10 +1590,10 @@
       <c r="D8" t="s">
         <v>9</v>
       </c>
-      <c r="G8" s="3">
+      <c r="G8" s="2">
         <v>44984</v>
       </c>
-      <c r="H8" s="3">
+      <c r="H8" s="2">
         <v>44987</v>
       </c>
     </row>
@@ -1605,10 +1610,10 @@
       <c r="F9" t="s">
         <v>37</v>
       </c>
-      <c r="G9" s="3">
+      <c r="G9" s="2">
         <v>44991</v>
       </c>
-      <c r="H9" s="4">
+      <c r="H9" s="3">
         <v>44994</v>
       </c>
     </row>
@@ -1616,19 +1621,19 @@
       <c r="A10">
         <v>11</v>
       </c>
-      <c r="B10" s="2" t="s">
+      <c r="B10" t="s">
         <v>10</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="C10" t="s">
         <v>22</v>
       </c>
-      <c r="D10" s="2" t="s">
+      <c r="D10" t="s">
         <v>10</v>
       </c>
-      <c r="G10" s="3">
+      <c r="G10" s="2">
         <v>44998</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H10" s="2">
         <v>45001</v>
       </c>
     </row>
@@ -1648,10 +1653,10 @@
       <c r="F11" t="s">
         <v>45</v>
       </c>
-      <c r="G11" s="3">
+      <c r="G11" s="2">
         <v>45005</v>
       </c>
-      <c r="H11" s="4">
+      <c r="H11" s="3">
         <v>45008</v>
       </c>
     </row>
@@ -1671,10 +1676,10 @@
       <c r="F12" t="s">
         <v>30</v>
       </c>
-      <c r="G12" s="3">
+      <c r="G12" s="2">
         <v>45012</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H12" s="2">
         <v>45015</v>
       </c>
     </row>
@@ -1688,10 +1693,10 @@
       <c r="E13" t="s">
         <v>31</v>
       </c>
-      <c r="G13" s="3">
+      <c r="G13" s="2">
         <v>45019</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="3">
         <v>45022</v>
       </c>
     </row>
@@ -1705,347 +1710,347 @@
       <c r="D14" t="s">
         <v>32</v>
       </c>
-      <c r="G14" s="4">
+      <c r="G14" s="3">
         <v>45026</v>
       </c>
-      <c r="H14" s="5">
+      <c r="H14" s="4">
         <v>45029</v>
       </c>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G15" s="3"/>
-      <c r="H15" s="5"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="4"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="G16" s="3"/>
-      <c r="H16" s="5"/>
-    </row>
-    <row r="17" spans="1:8" s="7" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="33" t="s">
+      <c r="G16" s="2"/>
+      <c r="H16" s="4"/>
+    </row>
+    <row r="17" spans="1:8" s="6" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="32" t="s">
         <v>47</v>
       </c>
-      <c r="C17" s="32" t="s">
+      <c r="C17" s="31" t="s">
         <v>48</v>
       </c>
-      <c r="D17" s="39"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="9"/>
+      <c r="D17" s="38"/>
+      <c r="G17" s="7"/>
+      <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="81" t="s">
+      <c r="A18" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="B18" s="24">
+      <c r="B18" s="23">
         <v>44942</v>
       </c>
-      <c r="C18" s="28">
+      <c r="C18" s="27">
         <v>44945</v>
       </c>
-      <c r="D18" s="40"/>
-    </row>
-    <row r="19" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="82"/>
-      <c r="B19" s="27" t="s">
+      <c r="D18" s="39"/>
+    </row>
+    <row r="19" spans="1:8" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="66"/>
+      <c r="B19" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C19" s="31" t="s">
+      <c r="C19" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="D19" s="41"/>
+      <c r="D19" s="40"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="82"/>
-      <c r="B20" s="24">
+      <c r="A20" s="66"/>
+      <c r="B20" s="23">
         <v>44949</v>
       </c>
-      <c r="C20" s="28">
+      <c r="C20" s="27">
         <v>44952</v>
       </c>
-      <c r="D20" s="40"/>
-    </row>
-    <row r="21" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="82"/>
-      <c r="B21" s="27" t="s">
+      <c r="D20" s="39"/>
+    </row>
+    <row r="21" spans="1:8" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A21" s="66"/>
+      <c r="B21" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C21" s="38" t="s">
+      <c r="C21" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="D21" s="41"/>
+      <c r="D21" s="40"/>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="82"/>
-      <c r="B22" s="24">
+      <c r="A22" s="66"/>
+      <c r="B22" s="23">
         <v>44956</v>
       </c>
-      <c r="C22" s="28">
+      <c r="C22" s="27">
         <v>44959</v>
       </c>
-      <c r="D22" s="40"/>
-    </row>
-    <row r="23" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="83"/>
-      <c r="B23" s="27" t="s">
+      <c r="D22" s="39"/>
+    </row>
+    <row r="23" spans="1:8" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="67"/>
+      <c r="B23" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="31" t="s">
+      <c r="C23" s="30" t="s">
         <v>7</v>
       </c>
-      <c r="D23" s="41"/>
+      <c r="D23" s="40"/>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="81" t="s">
+      <c r="A24" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="B24" s="26">
+      <c r="B24" s="25">
         <v>44963</v>
       </c>
-      <c r="C24" s="30">
+      <c r="C24" s="29">
         <v>44966</v>
       </c>
-      <c r="D24" s="40"/>
-    </row>
-    <row r="25" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="82"/>
-      <c r="B25" s="25" t="s">
+      <c r="D24" s="39"/>
+    </row>
+    <row r="25" spans="1:8" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="66"/>
+      <c r="B25" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C25" s="29" t="s">
+      <c r="C25" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="D25" s="41"/>
+      <c r="D25" s="40"/>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="82"/>
-      <c r="B26" s="24">
+      <c r="A26" s="66"/>
+      <c r="B26" s="23">
         <v>44970</v>
       </c>
-      <c r="C26" s="28">
+      <c r="C26" s="27">
         <v>44973</v>
       </c>
-      <c r="D26" s="40"/>
-    </row>
-    <row r="27" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="82"/>
-      <c r="B27" s="27" t="s">
+      <c r="D26" s="39"/>
+    </row>
+    <row r="27" spans="1:8" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="66"/>
+      <c r="B27" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="C27" s="31" t="s">
+      <c r="C27" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="D27" s="41"/>
+      <c r="D27" s="40"/>
     </row>
     <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="82"/>
-      <c r="B28" s="20">
+      <c r="A28" s="66"/>
+      <c r="B28" s="19">
         <v>44977</v>
       </c>
-      <c r="C28" s="15">
+      <c r="C28" s="14">
         <v>44980</v>
       </c>
-      <c r="D28" s="40"/>
-    </row>
-    <row r="29" spans="1:8" s="6" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="82"/>
-      <c r="B29" s="37" t="s">
+      <c r="D28" s="39"/>
+    </row>
+    <row r="29" spans="1:8" s="5" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="66"/>
+      <c r="B29" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="C29" s="37" t="s">
+      <c r="C29" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="D29" s="41"/>
+      <c r="D29" s="40"/>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="82"/>
-      <c r="B30" s="10">
+      <c r="A30" s="66"/>
+      <c r="B30" s="9">
         <v>44984</v>
       </c>
-      <c r="C30" s="13">
+      <c r="C30" s="12">
         <v>44987</v>
       </c>
-      <c r="D30" s="40"/>
-    </row>
-    <row r="31" spans="1:8" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="83"/>
-      <c r="B31" s="11" t="s">
+      <c r="D30" s="39"/>
+    </row>
+    <row r="31" spans="1:8" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="67"/>
+      <c r="B31" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C31" s="14" t="s">
+      <c r="C31" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="D31" s="41"/>
+      <c r="D31" s="40"/>
     </row>
     <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="81" t="s">
+      <c r="A32" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="B32" s="12">
+      <c r="B32" s="11">
         <v>44991</v>
       </c>
-      <c r="C32" s="20">
+      <c r="C32" s="19">
         <v>44994</v>
       </c>
-      <c r="D32" s="40"/>
-    </row>
-    <row r="33" spans="1:4" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="82"/>
-      <c r="B33" s="11" t="s">
+      <c r="D32" s="39"/>
+    </row>
+    <row r="33" spans="1:4" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="66"/>
+      <c r="B33" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="23" t="s">
+      <c r="C33" s="22" t="s">
         <v>50</v>
       </c>
-      <c r="D33" s="41"/>
+      <c r="D33" s="40"/>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="82"/>
-      <c r="B34" s="10">
+      <c r="A34" s="66"/>
+      <c r="B34" s="9">
         <v>44998</v>
       </c>
-      <c r="C34" s="13">
+      <c r="C34" s="12">
         <v>45001</v>
       </c>
-      <c r="D34" s="40"/>
-    </row>
-    <row r="35" spans="1:4" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="82"/>
-      <c r="B35" s="11" t="s">
+      <c r="D34" s="39"/>
+    </row>
+    <row r="35" spans="1:4" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="66"/>
+      <c r="B35" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C35" s="14" t="s">
+      <c r="C35" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="D35" s="41"/>
+      <c r="D35" s="40"/>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="82"/>
-      <c r="B36" s="16">
+      <c r="A36" s="66"/>
+      <c r="B36" s="15">
         <v>45005</v>
       </c>
-      <c r="C36" s="20">
+      <c r="C36" s="19">
         <v>45008</v>
       </c>
-      <c r="D36" s="40"/>
-    </row>
-    <row r="37" spans="1:4" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="82"/>
-      <c r="B37" s="17" t="s">
+      <c r="D36" s="39"/>
+    </row>
+    <row r="37" spans="1:4" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="66"/>
+      <c r="B37" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C37" s="21" t="s">
+      <c r="C37" s="20" t="s">
         <v>50</v>
       </c>
-      <c r="D37" s="41"/>
+      <c r="D37" s="40"/>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="82"/>
-      <c r="B38" s="19">
+      <c r="A38" s="66"/>
+      <c r="B38" s="18">
         <v>45012</v>
       </c>
-      <c r="C38" s="10">
+      <c r="C38" s="9">
         <v>45015</v>
       </c>
-      <c r="D38" s="40"/>
-    </row>
-    <row r="39" spans="1:4" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="83"/>
-      <c r="B39" s="18" t="s">
+      <c r="D38" s="39"/>
+    </row>
+    <row r="39" spans="1:4" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="67"/>
+      <c r="B39" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C39" s="11" t="s">
+      <c r="C39" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D39" s="41"/>
+      <c r="D39" s="40"/>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="81" t="s">
+      <c r="A40" s="65" t="s">
         <v>57</v>
       </c>
-      <c r="B40" s="34">
+      <c r="B40" s="33">
         <v>45019</v>
       </c>
-      <c r="C40" s="20">
+      <c r="C40" s="19">
         <v>45022</v>
       </c>
-      <c r="D40" s="40"/>
-    </row>
-    <row r="41" spans="1:4" s="6" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="82"/>
-      <c r="B41" s="35"/>
-      <c r="C41" s="23" t="s">
+      <c r="D40" s="39"/>
+    </row>
+    <row r="41" spans="1:4" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A41" s="66"/>
+      <c r="B41" s="34"/>
+      <c r="C41" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="D41" s="41"/>
+      <c r="D41" s="40"/>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="82"/>
-      <c r="B42" s="15">
+      <c r="A42" s="66"/>
+      <c r="B42" s="14">
         <v>45026</v>
       </c>
-      <c r="C42" s="12">
+      <c r="C42" s="11">
         <v>45029</v>
       </c>
-      <c r="D42" s="40"/>
-    </row>
-    <row r="43" spans="1:4" s="6" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="82"/>
-      <c r="B43" s="36" t="s">
+      <c r="D42" s="39"/>
+    </row>
+    <row r="43" spans="1:4" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A43" s="66"/>
+      <c r="B43" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="C43" s="22" t="s">
+      <c r="C43" s="21" t="s">
         <v>49</v>
       </c>
-      <c r="D43" s="41"/>
+      <c r="D43" s="40"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="82"/>
-      <c r="B44" s="84" t="s">
+      <c r="A44" s="66"/>
+      <c r="B44" s="68" t="s">
         <v>53</v>
       </c>
-      <c r="C44" s="85"/>
-      <c r="D44" s="40"/>
+      <c r="C44" s="69"/>
+      <c r="D44" s="39"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="82"/>
-      <c r="B45" s="86"/>
-      <c r="C45" s="87"/>
-      <c r="D45" s="40"/>
+      <c r="A45" s="66"/>
+      <c r="B45" s="70"/>
+      <c r="C45" s="71"/>
+      <c r="D45" s="39"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="83"/>
-      <c r="B46" s="88"/>
-      <c r="C46" s="89"/>
-      <c r="D46" s="40"/>
+      <c r="A46" s="67"/>
+      <c r="B46" s="72"/>
+      <c r="C46" s="73"/>
+      <c r="D46" s="39"/>
     </row>
     <row r="47" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="75" t="s">
+      <c r="A47" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="79">
+      <c r="B47" s="63">
         <v>45054</v>
       </c>
-      <c r="C47" s="80"/>
-      <c r="D47" s="40"/>
+      <c r="C47" s="64"/>
+      <c r="D47" s="39"/>
     </row>
     <row r="48" spans="1:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="76"/>
-      <c r="B48" s="77" t="s">
+      <c r="A48" s="60"/>
+      <c r="B48" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="C48" s="78"/>
-      <c r="D48" s="40"/>
+      <c r="C48" s="62"/>
+      <c r="D48" s="39"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A49" s="42"/>
-      <c r="B49" s="42"/>
-      <c r="C49" s="42"/>
-      <c r="D49" s="42"/>
+      <c r="A49" s="41"/>
+      <c r="B49" s="41"/>
+      <c r="C49" s="41"/>
+      <c r="D49" s="41"/>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="42"/>
-      <c r="B50" s="42"/>
-      <c r="C50" s="42"/>
-      <c r="D50" s="42"/>
+      <c r="A50" s="41"/>
+      <c r="B50" s="41"/>
+      <c r="C50" s="41"/>
+      <c r="D50" s="41"/>
     </row>
   </sheetData>
   <mergeCells count="8">
@@ -2067,8 +2072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1C02AE7A-CD84-44B4-BCAE-299F3ABE620B}">
   <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2079,278 +2084,276 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="70"/>
-      <c r="B1" s="71" t="s">
+      <c r="A1" s="54"/>
+      <c r="B1" s="55" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="72" t="s">
+      <c r="C1" s="56" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="94" t="s">
+      <c r="A2" s="78" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="43" t="s">
+      <c r="B2" s="83" t="s">
+        <v>68</v>
+      </c>
+      <c r="C2" s="84" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="79"/>
+      <c r="B3" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="C2" s="44" t="s">
+      <c r="C3" s="43" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="95"/>
-      <c r="B3" s="45" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="79"/>
+      <c r="B4" s="83" t="s">
+        <v>70</v>
+      </c>
+      <c r="C4" s="84" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="79"/>
+      <c r="B5" s="42" t="s">
+        <v>3</v>
+      </c>
+      <c r="C5" s="44" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="79"/>
+      <c r="B6" s="83" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" s="84" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="80"/>
+      <c r="B7" s="42" t="s">
+        <v>7</v>
+      </c>
+      <c r="C7" s="43" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="78" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="85" t="s">
+        <v>74</v>
+      </c>
+      <c r="C8" s="86" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="79"/>
+      <c r="B9" s="45" t="s">
+        <v>8</v>
+      </c>
+      <c r="C9" s="46" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="79"/>
+      <c r="B10" s="83" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" s="84" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="79"/>
+      <c r="B11" s="42" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="43" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="79"/>
+      <c r="B12" s="87" t="s">
+        <v>78</v>
+      </c>
+      <c r="C12" s="88" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="79"/>
+      <c r="B13" s="47" t="s">
+        <v>59</v>
+      </c>
+      <c r="C13" s="47" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="79"/>
+      <c r="B14" s="89" t="s">
+        <v>80</v>
+      </c>
+      <c r="C14" s="90" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="80"/>
+      <c r="B15" s="48" t="s">
+        <v>43</v>
+      </c>
+      <c r="C15" s="49" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="78" t="s">
+        <v>56</v>
+      </c>
+      <c r="B16" s="99" t="s">
+        <v>83</v>
+      </c>
+      <c r="C16" s="89" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="79"/>
+      <c r="B17" s="50" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" s="48" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="79"/>
+      <c r="B18" s="89" t="s">
+        <v>82</v>
+      </c>
+      <c r="C18" s="90" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="79"/>
+      <c r="B19" s="48" t="s">
+        <v>64</v>
+      </c>
+      <c r="C19" s="49" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="79"/>
+      <c r="B20" s="92" t="s">
         <v>87</v>
       </c>
-      <c r="C3" s="46" t="s">
+      <c r="C20" s="89" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="79"/>
+      <c r="B21" s="51" t="s">
+        <v>11</v>
+      </c>
+      <c r="C21" s="98" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="79"/>
+      <c r="B22" s="93" t="s">
+        <v>89</v>
+      </c>
+      <c r="C22" s="87" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="95"/>
-      <c r="B4" s="43" t="s">
-        <v>63</v>
-      </c>
-      <c r="C4" s="44" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="95"/>
-      <c r="B5" s="45" t="s">
-        <v>3</v>
-      </c>
-      <c r="C5" s="47" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="95"/>
-      <c r="B6" s="43" t="s">
-        <v>65</v>
-      </c>
-      <c r="C6" s="44" t="s">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="80"/>
+      <c r="B23" s="94" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="95" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="78" t="s">
+        <v>57</v>
+      </c>
+      <c r="B24" s="96" t="s">
+        <v>91</v>
+      </c>
+      <c r="C24" s="97" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="79"/>
+      <c r="B25" s="94" t="s">
+        <v>44</v>
+      </c>
+      <c r="C25" s="52" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A26" s="79"/>
+      <c r="B26" s="90" t="s">
+        <v>93</v>
+      </c>
+      <c r="C26" s="91" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A27" s="79"/>
+      <c r="B27" s="48" t="s">
         <v>66</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="96"/>
-      <c r="B7" s="45" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="46" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="94" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="48" t="s">
+      <c r="C27" s="53" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A28" s="79"/>
+      <c r="B28" s="57" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="58"/>
+    </row>
+    <row r="29" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="A29" s="81"/>
+      <c r="B29" s="74" t="s">
         <v>67</v>
       </c>
-      <c r="C8" s="49" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="95"/>
-      <c r="B9" s="50" t="s">
-        <v>8</v>
-      </c>
-      <c r="C9" s="51" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="95"/>
-      <c r="B10" s="43" t="s">
-        <v>69</v>
-      </c>
-      <c r="C10" s="44" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="95"/>
-      <c r="B11" s="45" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="46" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="95"/>
-      <c r="B12" s="52" t="s">
-        <v>71</v>
-      </c>
-      <c r="C12" s="53" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="95"/>
-      <c r="B13" s="54" t="s">
-        <v>59</v>
-      </c>
-      <c r="C13" s="54" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="95"/>
-      <c r="B14" s="55" t="s">
-        <v>73</v>
-      </c>
-      <c r="C14" s="56" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="96"/>
-      <c r="B15" s="57" t="s">
-        <v>43</v>
-      </c>
-      <c r="C15" s="58" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="94" t="s">
-        <v>56</v>
-      </c>
-      <c r="B16" s="59" t="s">
-        <v>75</v>
-      </c>
-      <c r="C16" s="52" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="95"/>
-      <c r="B17" s="57" t="s">
-        <v>43</v>
-      </c>
-      <c r="C17" s="60" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="95"/>
-      <c r="B18" s="55" t="s">
-        <v>77</v>
-      </c>
-      <c r="C18" s="56" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="95"/>
-      <c r="B19" s="57" t="s">
-        <v>91</v>
-      </c>
-      <c r="C19" s="58" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="95"/>
-      <c r="B20" s="61" t="s">
-        <v>79</v>
-      </c>
-      <c r="C20" s="52" t="s">
-        <v>90</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="95"/>
-      <c r="B21" s="62" t="s">
-        <v>11</v>
-      </c>
-      <c r="C21" s="63" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="95"/>
-      <c r="B22" s="64" t="s">
-        <v>82</v>
-      </c>
-      <c r="C22" s="55" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="96"/>
-      <c r="B23" s="65" t="s">
-        <v>11</v>
-      </c>
-      <c r="C23" s="57" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="94" t="s">
-        <v>57</v>
-      </c>
-      <c r="B24" s="66" t="s">
-        <v>80</v>
-      </c>
-      <c r="C24" s="52" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="95"/>
-      <c r="B25" s="67" t="s">
-        <v>44</v>
-      </c>
-      <c r="C25" s="60" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="95"/>
-      <c r="B26" s="53" t="s">
-        <v>85</v>
-      </c>
-      <c r="C26" s="59" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="95"/>
-      <c r="B27" s="68" t="s">
-        <v>44</v>
-      </c>
-      <c r="C27" s="69" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="95"/>
-      <c r="B28" s="73" t="s">
-        <v>53</v>
-      </c>
-      <c r="C28" s="74"/>
-    </row>
-    <row r="29" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="97" t="s">
-        <v>51</v>
-      </c>
-      <c r="B29" s="90" t="s">
-        <v>86</v>
-      </c>
-      <c r="C29" s="91"/>
+      <c r="C29" s="75"/>
     </row>
     <row r="30" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="98"/>
-      <c r="B30" s="92" t="s">
+      <c r="A30" s="82"/>
+      <c r="B30" s="76" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="93"/>
+      <c r="C30" s="77"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2371,8 +2374,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A780E3C1-B692-48F8-988B-66A9EFA8823C}">
   <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E5" sqref="E5"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2382,286 +2385,286 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" s="7"/>
-      <c r="B1" s="33" t="s">
+      <c r="A1" s="6"/>
+      <c r="B1" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="32" t="s">
+      <c r="C1" s="31" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="81" t="s">
+      <c r="A2" s="65" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="24">
+      <c r="B2" s="23">
         <v>44942</v>
       </c>
-      <c r="C2" s="28">
+      <c r="C2" s="27">
         <v>44945</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="82"/>
-      <c r="B3" s="27" t="s">
+      <c r="A3" s="66"/>
+      <c r="B3" s="26" t="s">
         <v>40</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="30" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="82"/>
-      <c r="B4" s="24">
+      <c r="A4" s="66"/>
+      <c r="B4" s="23">
         <v>44949</v>
       </c>
-      <c r="C4" s="28">
+      <c r="C4" s="27">
         <v>44952</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="82"/>
-      <c r="B5" s="27" t="s">
+      <c r="A5" s="66"/>
+      <c r="B5" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="38" t="s">
+      <c r="C5" s="37" t="s">
         <v>58</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="82"/>
-      <c r="B6" s="24">
+      <c r="A6" s="66"/>
+      <c r="B6" s="23">
         <v>44956</v>
       </c>
-      <c r="C6" s="28">
+      <c r="C6" s="27">
         <v>44959</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="83"/>
-      <c r="B7" s="27" t="s">
+      <c r="A7" s="67"/>
+      <c r="B7" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="31" t="s">
+      <c r="C7" s="30" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="81" t="s">
+      <c r="A8" s="65" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="26">
+      <c r="B8" s="25">
         <v>44963</v>
       </c>
-      <c r="C8" s="30">
+      <c r="C8" s="29">
         <v>44966</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="82"/>
-      <c r="B9" s="25" t="s">
+      <c r="A9" s="66"/>
+      <c r="B9" s="24" t="s">
         <v>8</v>
       </c>
-      <c r="C9" s="29" t="s">
+      <c r="C9" s="28" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="82"/>
-      <c r="B10" s="24">
+      <c r="A10" s="66"/>
+      <c r="B10" s="23">
         <v>44970</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C10" s="27">
         <v>44973</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="82"/>
-      <c r="B11" s="27" t="s">
+      <c r="A11" s="66"/>
+      <c r="B11" s="26" t="s">
         <v>42</v>
       </c>
-      <c r="C11" s="31" t="s">
+      <c r="C11" s="30" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="82"/>
-      <c r="B12" s="20">
+      <c r="A12" s="66"/>
+      <c r="B12" s="19">
         <v>44977</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="14">
         <v>44980</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="82"/>
-      <c r="B13" s="37" t="s">
+      <c r="A13" s="66"/>
+      <c r="B13" s="36" t="s">
         <v>59</v>
       </c>
-      <c r="C13" s="37" t="s">
+      <c r="C13" s="36" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="82"/>
-      <c r="B14" s="10">
+      <c r="A14" s="66"/>
+      <c r="B14" s="9">
         <v>44984</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="12">
         <v>44987</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="83"/>
-      <c r="B15" s="11" t="s">
+      <c r="A15" s="67"/>
+      <c r="B15" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="13" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="81" t="s">
+      <c r="A16" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="12">
+      <c r="B16" s="11">
         <v>44991</v>
       </c>
-      <c r="C16" s="20">
+      <c r="C16" s="19">
         <v>44994</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="82"/>
-      <c r="B17" s="11" t="s">
+      <c r="A17" s="66"/>
+      <c r="B17" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C17" s="23" t="s">
+      <c r="C17" s="22" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="82"/>
-      <c r="B18" s="10">
+      <c r="A18" s="66"/>
+      <c r="B18" s="9">
         <v>44998</v>
       </c>
-      <c r="C18" s="13">
+      <c r="C18" s="12">
         <v>45001</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="82"/>
-      <c r="B19" s="11" t="s">
+      <c r="A19" s="66"/>
+      <c r="B19" s="10" t="s">
         <v>43</v>
       </c>
-      <c r="C19" s="14" t="s">
+      <c r="C19" s="13" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="82"/>
-      <c r="B20" s="16">
+      <c r="A20" s="66"/>
+      <c r="B20" s="15">
         <v>45005</v>
       </c>
-      <c r="C20" s="20">
+      <c r="C20" s="19">
         <v>45008</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="82"/>
-      <c r="B21" s="17" t="s">
+      <c r="A21" s="66"/>
+      <c r="B21" s="16" t="s">
         <v>46</v>
       </c>
-      <c r="C21" s="21" t="s">
+      <c r="C21" s="20" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="82"/>
-      <c r="B22" s="19">
+      <c r="A22" s="66"/>
+      <c r="B22" s="18">
         <v>45012</v>
       </c>
-      <c r="C22" s="10">
+      <c r="C22" s="9">
         <v>45015</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="83"/>
-      <c r="B23" s="18" t="s">
+      <c r="A23" s="67"/>
+      <c r="B23" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="C23" s="11" t="s">
+      <c r="C23" s="10" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="81" t="s">
+      <c r="A24" s="65" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="34">
+      <c r="B24" s="33">
         <v>45019</v>
       </c>
-      <c r="C24" s="20">
+      <c r="C24" s="19">
         <v>45022</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="82"/>
-      <c r="B25" s="35"/>
-      <c r="C25" s="23" t="s">
+      <c r="A25" s="66"/>
+      <c r="B25" s="34"/>
+      <c r="C25" s="22" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="82"/>
-      <c r="B26" s="15">
+      <c r="A26" s="66"/>
+      <c r="B26" s="14">
         <v>45026</v>
       </c>
-      <c r="C26" s="12">
+      <c r="C26" s="11">
         <v>45029</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="82"/>
-      <c r="B27" s="36" t="s">
+      <c r="A27" s="66"/>
+      <c r="B27" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="C27" s="22" t="s">
+      <c r="C27" s="21" t="s">
         <v>49</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="82"/>
-      <c r="B28" s="84" t="s">
+      <c r="A28" s="66"/>
+      <c r="B28" s="68" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="85"/>
+      <c r="C28" s="69"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="82"/>
-      <c r="B29" s="86"/>
-      <c r="C29" s="87"/>
+      <c r="A29" s="66"/>
+      <c r="B29" s="70"/>
+      <c r="C29" s="71"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="83"/>
-      <c r="B30" s="88"/>
-      <c r="C30" s="89"/>
+      <c r="A30" s="67"/>
+      <c r="B30" s="72"/>
+      <c r="C30" s="73"/>
     </row>
     <row r="31" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="75" t="s">
+      <c r="A31" s="59" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="79">
+      <c r="B31" s="63">
         <v>45054</v>
       </c>
-      <c r="C31" s="80"/>
+      <c r="C31" s="64"/>
     </row>
     <row r="32" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A32" s="76"/>
-      <c r="B32" s="77" t="s">
+      <c r="A32" s="60"/>
+      <c r="B32" s="61" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="78"/>
+      <c r="C32" s="62"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>

<commit_message>
updated monday lecture hours
</commit_message>
<xml_diff>
--- a/lecturePlan.xlsx
+++ b/lecturePlan.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\s15052\Documents\Teaching\BAN430\BAN430_book\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9615B9EA-DD64-495A-8B60-6412B620A873}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB848768-79B4-4E64-B3AE-CAACFA3332F4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="2" xr2:uid="{DEDCCCE6-C2B3-4C3C-BD8B-2E3EEC4135F8}"/>
+    <workbookView xWindow="3720" yWindow="3720" windowWidth="21600" windowHeight="11295" activeTab="2" xr2:uid="{DEDCCCE6-C2B3-4C3C-BD8B-2E3EEC4135F8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="94">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="228" uniqueCount="95">
   <si>
     <t>Week number</t>
   </si>
@@ -318,6 +318,9 @@
   </si>
   <si>
     <t>08.04.2024</t>
+  </si>
+  <si>
+    <t>Monday 10:15-12:00</t>
   </si>
 </sst>
 </file>
@@ -730,78 +733,6 @@
     <xf numFmtId="49" fontId="7" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="8" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="8" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="9" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="49" fontId="1" fillId="4" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -842,7 +773,7 @@
     <xf numFmtId="49" fontId="6" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="6" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="49" fontId="5" fillId="4" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -850,6 +781,78 @@
     </xf>
     <xf numFmtId="49" fontId="6" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="8" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="8" fillId="5" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="5" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="5" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="9" fillId="5" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1737,7 +1740,7 @@
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="65" t="s">
+      <c r="A18" s="82" t="s">
         <v>54</v>
       </c>
       <c r="B18" s="23">
@@ -1749,7 +1752,7 @@
       <c r="D18" s="39"/>
     </row>
     <row r="19" spans="1:8" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="66"/>
+      <c r="A19" s="83"/>
       <c r="B19" s="26" t="s">
         <v>40</v>
       </c>
@@ -1759,7 +1762,7 @@
       <c r="D19" s="40"/>
     </row>
     <row r="20" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="66"/>
+      <c r="A20" s="83"/>
       <c r="B20" s="23">
         <v>44949</v>
       </c>
@@ -1769,7 +1772,7 @@
       <c r="D20" s="39"/>
     </row>
     <row r="21" spans="1:8" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="66"/>
+      <c r="A21" s="83"/>
       <c r="B21" s="26" t="s">
         <v>3</v>
       </c>
@@ -1779,7 +1782,7 @@
       <c r="D21" s="40"/>
     </row>
     <row r="22" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="66"/>
+      <c r="A22" s="83"/>
       <c r="B22" s="23">
         <v>44956</v>
       </c>
@@ -1789,7 +1792,7 @@
       <c r="D22" s="39"/>
     </row>
     <row r="23" spans="1:8" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="67"/>
+      <c r="A23" s="84"/>
       <c r="B23" s="26" t="s">
         <v>7</v>
       </c>
@@ -1799,7 +1802,7 @@
       <c r="D23" s="40"/>
     </row>
     <row r="24" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="65" t="s">
+      <c r="A24" s="82" t="s">
         <v>55</v>
       </c>
       <c r="B24" s="25">
@@ -1811,7 +1814,7 @@
       <c r="D24" s="39"/>
     </row>
     <row r="25" spans="1:8" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="66"/>
+      <c r="A25" s="83"/>
       <c r="B25" s="24" t="s">
         <v>8</v>
       </c>
@@ -1821,7 +1824,7 @@
       <c r="D25" s="40"/>
     </row>
     <row r="26" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="66"/>
+      <c r="A26" s="83"/>
       <c r="B26" s="23">
         <v>44970</v>
       </c>
@@ -1831,7 +1834,7 @@
       <c r="D26" s="39"/>
     </row>
     <row r="27" spans="1:8" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="66"/>
+      <c r="A27" s="83"/>
       <c r="B27" s="26" t="s">
         <v>42</v>
       </c>
@@ -1841,7 +1844,7 @@
       <c r="D27" s="40"/>
     </row>
     <row r="28" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="66"/>
+      <c r="A28" s="83"/>
       <c r="B28" s="19">
         <v>44977</v>
       </c>
@@ -1851,7 +1854,7 @@
       <c r="D28" s="39"/>
     </row>
     <row r="29" spans="1:8" s="5" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="66"/>
+      <c r="A29" s="83"/>
       <c r="B29" s="36" t="s">
         <v>59</v>
       </c>
@@ -1861,7 +1864,7 @@
       <c r="D29" s="40"/>
     </row>
     <row r="30" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="66"/>
+      <c r="A30" s="83"/>
       <c r="B30" s="9">
         <v>44984</v>
       </c>
@@ -1871,7 +1874,7 @@
       <c r="D30" s="39"/>
     </row>
     <row r="31" spans="1:8" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A31" s="67"/>
+      <c r="A31" s="84"/>
       <c r="B31" s="10" t="s">
         <v>43</v>
       </c>
@@ -1881,7 +1884,7 @@
       <c r="D31" s="40"/>
     </row>
     <row r="32" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A32" s="65" t="s">
+      <c r="A32" s="82" t="s">
         <v>56</v>
       </c>
       <c r="B32" s="11">
@@ -1893,7 +1896,7 @@
       <c r="D32" s="39"/>
     </row>
     <row r="33" spans="1:4" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A33" s="66"/>
+      <c r="A33" s="83"/>
       <c r="B33" s="10" t="s">
         <v>43</v>
       </c>
@@ -1903,7 +1906,7 @@
       <c r="D33" s="40"/>
     </row>
     <row r="34" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A34" s="66"/>
+      <c r="A34" s="83"/>
       <c r="B34" s="9">
         <v>44998</v>
       </c>
@@ -1913,7 +1916,7 @@
       <c r="D34" s="39"/>
     </row>
     <row r="35" spans="1:4" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A35" s="66"/>
+      <c r="A35" s="83"/>
       <c r="B35" s="10" t="s">
         <v>43</v>
       </c>
@@ -1923,7 +1926,7 @@
       <c r="D35" s="40"/>
     </row>
     <row r="36" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A36" s="66"/>
+      <c r="A36" s="83"/>
       <c r="B36" s="15">
         <v>45005</v>
       </c>
@@ -1933,7 +1936,7 @@
       <c r="D36" s="39"/>
     </row>
     <row r="37" spans="1:4" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A37" s="66"/>
+      <c r="A37" s="83"/>
       <c r="B37" s="16" t="s">
         <v>46</v>
       </c>
@@ -1943,7 +1946,7 @@
       <c r="D37" s="40"/>
     </row>
     <row r="38" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A38" s="66"/>
+      <c r="A38" s="83"/>
       <c r="B38" s="18">
         <v>45012</v>
       </c>
@@ -1953,7 +1956,7 @@
       <c r="D38" s="39"/>
     </row>
     <row r="39" spans="1:4" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="67"/>
+      <c r="A39" s="84"/>
       <c r="B39" s="17" t="s">
         <v>11</v>
       </c>
@@ -1963,7 +1966,7 @@
       <c r="D39" s="40"/>
     </row>
     <row r="40" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A40" s="65" t="s">
+      <c r="A40" s="82" t="s">
         <v>57</v>
       </c>
       <c r="B40" s="33">
@@ -1975,7 +1978,7 @@
       <c r="D40" s="39"/>
     </row>
     <row r="41" spans="1:4" s="5" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A41" s="66"/>
+      <c r="A41" s="83"/>
       <c r="B41" s="34"/>
       <c r="C41" s="22" t="s">
         <v>44</v>
@@ -1983,7 +1986,7 @@
       <c r="D41" s="40"/>
     </row>
     <row r="42" spans="1:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="66"/>
+      <c r="A42" s="83"/>
       <c r="B42" s="14">
         <v>45026</v>
       </c>
@@ -1993,7 +1996,7 @@
       <c r="D42" s="39"/>
     </row>
     <row r="43" spans="1:4" s="5" customFormat="1" ht="31.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="66"/>
+      <c r="A43" s="83"/>
       <c r="B43" s="35" t="s">
         <v>44</v>
       </c>
@@ -2003,41 +2006,41 @@
       <c r="D43" s="40"/>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" s="66"/>
-      <c r="B44" s="68" t="s">
+      <c r="A44" s="83"/>
+      <c r="B44" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="C44" s="69"/>
+      <c r="C44" s="86"/>
       <c r="D44" s="39"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A45" s="66"/>
-      <c r="B45" s="70"/>
-      <c r="C45" s="71"/>
+      <c r="A45" s="83"/>
+      <c r="B45" s="87"/>
+      <c r="C45" s="88"/>
       <c r="D45" s="39"/>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="67"/>
-      <c r="B46" s="72"/>
-      <c r="C46" s="73"/>
+      <c r="A46" s="84"/>
+      <c r="B46" s="89"/>
+      <c r="C46" s="90"/>
       <c r="D46" s="39"/>
     </row>
     <row r="47" spans="1:4" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A47" s="59" t="s">
+      <c r="A47" s="76" t="s">
         <v>51</v>
       </c>
-      <c r="B47" s="63">
+      <c r="B47" s="80">
         <v>45054</v>
       </c>
-      <c r="C47" s="64"/>
+      <c r="C47" s="81"/>
       <c r="D47" s="39"/>
     </row>
     <row r="48" spans="1:4" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="60"/>
-      <c r="B48" s="61" t="s">
+      <c r="A48" s="77"/>
+      <c r="B48" s="78" t="s">
         <v>52</v>
       </c>
-      <c r="C48" s="62"/>
+      <c r="C48" s="79"/>
       <c r="D48" s="39"/>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
@@ -2073,7 +2076,7 @@
   <dimension ref="A1:C30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2086,25 +2089,25 @@
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="54"/>
       <c r="B1" s="55" t="s">
-        <v>34</v>
+        <v>94</v>
       </c>
       <c r="C1" s="56" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="78" t="s">
+      <c r="A2" s="95" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="83" t="s">
+      <c r="B2" s="59" t="s">
         <v>68</v>
       </c>
-      <c r="C2" s="84" t="s">
+      <c r="C2" s="60" t="s">
         <v>69</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="79"/>
+      <c r="A3" s="96"/>
       <c r="B3" s="42" t="s">
         <v>61</v>
       </c>
@@ -2113,16 +2116,16 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="79"/>
-      <c r="B4" s="83" t="s">
+      <c r="A4" s="96"/>
+      <c r="B4" s="59" t="s">
         <v>70</v>
       </c>
-      <c r="C4" s="84" t="s">
+      <c r="C4" s="60" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="79"/>
+      <c r="A5" s="96"/>
       <c r="B5" s="42" t="s">
         <v>3</v>
       </c>
@@ -2131,16 +2134,16 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="79"/>
-      <c r="B6" s="83" t="s">
+      <c r="A6" s="96"/>
+      <c r="B6" s="59" t="s">
         <v>72</v>
       </c>
-      <c r="C6" s="84" t="s">
+      <c r="C6" s="60" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="80"/>
+      <c r="A7" s="97"/>
       <c r="B7" s="42" t="s">
         <v>7</v>
       </c>
@@ -2149,18 +2152,18 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="78" t="s">
+      <c r="A8" s="95" t="s">
         <v>55</v>
       </c>
-      <c r="B8" s="85" t="s">
+      <c r="B8" s="61" t="s">
         <v>74</v>
       </c>
-      <c r="C8" s="86" t="s">
+      <c r="C8" s="62" t="s">
         <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="79"/>
+      <c r="A9" s="96"/>
       <c r="B9" s="45" t="s">
         <v>8</v>
       </c>
@@ -2169,16 +2172,16 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="79"/>
-      <c r="B10" s="83" t="s">
+      <c r="A10" s="96"/>
+      <c r="B10" s="59" t="s">
         <v>76</v>
       </c>
-      <c r="C10" s="84" t="s">
+      <c r="C10" s="60" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="79"/>
+      <c r="A11" s="96"/>
       <c r="B11" s="42" t="s">
         <v>42</v>
       </c>
@@ -2187,16 +2190,16 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="79"/>
-      <c r="B12" s="87" t="s">
+      <c r="A12" s="96"/>
+      <c r="B12" s="63" t="s">
         <v>78</v>
       </c>
-      <c r="C12" s="88" t="s">
+      <c r="C12" s="64" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="79"/>
+      <c r="A13" s="96"/>
       <c r="B13" s="47" t="s">
         <v>59</v>
       </c>
@@ -2205,16 +2208,16 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="79"/>
-      <c r="B14" s="89" t="s">
+      <c r="A14" s="96"/>
+      <c r="B14" s="65" t="s">
         <v>80</v>
       </c>
-      <c r="C14" s="90" t="s">
+      <c r="C14" s="66" t="s">
         <v>81</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="80"/>
+      <c r="A15" s="97"/>
       <c r="B15" s="48" t="s">
         <v>43</v>
       </c>
@@ -2223,18 +2226,18 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="78" t="s">
+      <c r="A16" s="95" t="s">
         <v>56</v>
       </c>
-      <c r="B16" s="99" t="s">
+      <c r="B16" s="75" t="s">
         <v>83</v>
       </c>
-      <c r="C16" s="89" t="s">
+      <c r="C16" s="65" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="79"/>
+      <c r="A17" s="96"/>
       <c r="B17" s="50" t="s">
         <v>50</v>
       </c>
@@ -2243,16 +2246,16 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="79"/>
-      <c r="B18" s="89" t="s">
+      <c r="A18" s="96"/>
+      <c r="B18" s="65" t="s">
         <v>82</v>
       </c>
-      <c r="C18" s="90" t="s">
+      <c r="C18" s="66" t="s">
         <v>85</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="79"/>
+      <c r="A19" s="96"/>
       <c r="B19" s="48" t="s">
         <v>64</v>
       </c>
@@ -2261,55 +2264,55 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="79"/>
-      <c r="B20" s="92" t="s">
+      <c r="A20" s="96"/>
+      <c r="B20" s="68" t="s">
         <v>87</v>
       </c>
-      <c r="C20" s="89" t="s">
+      <c r="C20" s="65" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="79"/>
+      <c r="A21" s="96"/>
       <c r="B21" s="51" t="s">
         <v>11</v>
       </c>
-      <c r="C21" s="98" t="s">
+      <c r="C21" s="74" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="79"/>
-      <c r="B22" s="93" t="s">
+      <c r="A22" s="96"/>
+      <c r="B22" s="69" t="s">
         <v>89</v>
       </c>
-      <c r="C22" s="87" t="s">
+      <c r="C22" s="63" t="s">
         <v>88</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="80"/>
-      <c r="B23" s="94" t="s">
+      <c r="A23" s="97"/>
+      <c r="B23" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="C23" s="95" t="s">
+      <c r="C23" s="71" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="78" t="s">
+      <c r="A24" s="95" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="96" t="s">
+      <c r="B24" s="72" t="s">
         <v>91</v>
       </c>
-      <c r="C24" s="97" t="s">
+      <c r="C24" s="73" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="79"/>
-      <c r="B25" s="94" t="s">
+      <c r="A25" s="96"/>
+      <c r="B25" s="70" t="s">
         <v>44</v>
       </c>
       <c r="C25" s="52" t="s">
@@ -2317,16 +2320,16 @@
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="79"/>
-      <c r="B26" s="90" t="s">
+      <c r="A26" s="96"/>
+      <c r="B26" s="66" t="s">
         <v>93</v>
       </c>
-      <c r="C26" s="91" t="s">
+      <c r="C26" s="67" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="79"/>
+      <c r="A27" s="96"/>
       <c r="B27" s="48" t="s">
         <v>66</v>
       </c>
@@ -2335,25 +2338,25 @@
       </c>
     </row>
     <row r="28" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="79"/>
+      <c r="A28" s="96"/>
       <c r="B28" s="57" t="s">
         <v>53</v>
       </c>
       <c r="C28" s="58"/>
     </row>
     <row r="29" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A29" s="81"/>
-      <c r="B29" s="74" t="s">
+      <c r="A29" s="98"/>
+      <c r="B29" s="91" t="s">
         <v>67</v>
       </c>
-      <c r="C29" s="75"/>
+      <c r="C29" s="92"/>
     </row>
     <row r="30" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A30" s="82"/>
-      <c r="B30" s="76" t="s">
+      <c r="A30" s="99"/>
+      <c r="B30" s="93" t="s">
         <v>52</v>
       </c>
-      <c r="C30" s="77"/>
+      <c r="C30" s="94"/>
     </row>
   </sheetData>
   <mergeCells count="7">
@@ -2394,7 +2397,7 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" s="65" t="s">
+      <c r="A2" s="82" t="s">
         <v>54</v>
       </c>
       <c r="B2" s="23">
@@ -2405,7 +2408,7 @@
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" s="66"/>
+      <c r="A3" s="83"/>
       <c r="B3" s="26" t="s">
         <v>40</v>
       </c>
@@ -2414,7 +2417,7 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="66"/>
+      <c r="A4" s="83"/>
       <c r="B4" s="23">
         <v>44949</v>
       </c>
@@ -2423,7 +2426,7 @@
       </c>
     </row>
     <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="66"/>
+      <c r="A5" s="83"/>
       <c r="B5" s="26" t="s">
         <v>3</v>
       </c>
@@ -2432,7 +2435,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="66"/>
+      <c r="A6" s="83"/>
       <c r="B6" s="23">
         <v>44956</v>
       </c>
@@ -2441,7 +2444,7 @@
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="67"/>
+      <c r="A7" s="84"/>
       <c r="B7" s="26" t="s">
         <v>7</v>
       </c>
@@ -2450,7 +2453,7 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="65" t="s">
+      <c r="A8" s="82" t="s">
         <v>55</v>
       </c>
       <c r="B8" s="25">
@@ -2461,7 +2464,7 @@
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="66"/>
+      <c r="A9" s="83"/>
       <c r="B9" s="24" t="s">
         <v>8</v>
       </c>
@@ -2470,7 +2473,7 @@
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="66"/>
+      <c r="A10" s="83"/>
       <c r="B10" s="23">
         <v>44970</v>
       </c>
@@ -2479,7 +2482,7 @@
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="66"/>
+      <c r="A11" s="83"/>
       <c r="B11" s="26" t="s">
         <v>42</v>
       </c>
@@ -2488,7 +2491,7 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="66"/>
+      <c r="A12" s="83"/>
       <c r="B12" s="19">
         <v>44977</v>
       </c>
@@ -2497,7 +2500,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A13" s="66"/>
+      <c r="A13" s="83"/>
       <c r="B13" s="36" t="s">
         <v>59</v>
       </c>
@@ -2506,7 +2509,7 @@
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="66"/>
+      <c r="A14" s="83"/>
       <c r="B14" s="9">
         <v>44984</v>
       </c>
@@ -2515,7 +2518,7 @@
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="67"/>
+      <c r="A15" s="84"/>
       <c r="B15" s="10" t="s">
         <v>43</v>
       </c>
@@ -2524,7 +2527,7 @@
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="65" t="s">
+      <c r="A16" s="82" t="s">
         <v>56</v>
       </c>
       <c r="B16" s="11">
@@ -2535,7 +2538,7 @@
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="66"/>
+      <c r="A17" s="83"/>
       <c r="B17" s="10" t="s">
         <v>43</v>
       </c>
@@ -2544,7 +2547,7 @@
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="66"/>
+      <c r="A18" s="83"/>
       <c r="B18" s="9">
         <v>44998</v>
       </c>
@@ -2553,7 +2556,7 @@
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="66"/>
+      <c r="A19" s="83"/>
       <c r="B19" s="10" t="s">
         <v>43</v>
       </c>
@@ -2562,7 +2565,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="66"/>
+      <c r="A20" s="83"/>
       <c r="B20" s="15">
         <v>45005</v>
       </c>
@@ -2571,7 +2574,7 @@
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="66"/>
+      <c r="A21" s="83"/>
       <c r="B21" s="16" t="s">
         <v>46</v>
       </c>
@@ -2580,7 +2583,7 @@
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="66"/>
+      <c r="A22" s="83"/>
       <c r="B22" s="18">
         <v>45012</v>
       </c>
@@ -2589,7 +2592,7 @@
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="67"/>
+      <c r="A23" s="84"/>
       <c r="B23" s="17" t="s">
         <v>11</v>
       </c>
@@ -2598,7 +2601,7 @@
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="65" t="s">
+      <c r="A24" s="82" t="s">
         <v>57</v>
       </c>
       <c r="B24" s="33">
@@ -2609,14 +2612,14 @@
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="66"/>
+      <c r="A25" s="83"/>
       <c r="B25" s="34"/>
       <c r="C25" s="22" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="66"/>
+      <c r="A26" s="83"/>
       <c r="B26" s="14">
         <v>45026</v>
       </c>
@@ -2625,7 +2628,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="66"/>
+      <c r="A27" s="83"/>
       <c r="B27" s="35" t="s">
         <v>44</v>
       </c>
@@ -2634,37 +2637,37 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="66"/>
-      <c r="B28" s="68" t="s">
+      <c r="A28" s="83"/>
+      <c r="B28" s="85" t="s">
         <v>53</v>
       </c>
-      <c r="C28" s="69"/>
+      <c r="C28" s="86"/>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="66"/>
-      <c r="B29" s="70"/>
-      <c r="C29" s="71"/>
+      <c r="A29" s="83"/>
+      <c r="B29" s="87"/>
+      <c r="C29" s="88"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="67"/>
-      <c r="B30" s="72"/>
-      <c r="C30" s="73"/>
+      <c r="A30" s="84"/>
+      <c r="B30" s="89"/>
+      <c r="C30" s="90"/>
     </row>
     <row r="31" spans="1:3" ht="18.75" x14ac:dyDescent="0.25">
-      <c r="A31" s="59" t="s">
+      <c r="A31" s="76" t="s">
         <v>51</v>
       </c>
-      <c r="B31" s="63">
+      <c r="B31" s="80">
         <v>45054</v>
       </c>
-      <c r="C31" s="64"/>
+      <c r="C31" s="81"/>
     </row>
     <row r="32" spans="1:3" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A32" s="60"/>
-      <c r="B32" s="61" t="s">
+      <c r="A32" s="77"/>
+      <c r="B32" s="78" t="s">
         <v>52</v>
       </c>
-      <c r="C32" s="62"/>
+      <c r="C32" s="79"/>
     </row>
   </sheetData>
   <mergeCells count="8">

</xml_diff>